<commit_message>
update note about debug
</commit_message>
<xml_diff>
--- a/项目笔记/8_无人值守/无人值守问题和需求备注.xlsx
+++ b/项目笔记/8_无人值守/无人值守问题和需求备注.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Computer\project-note\项目笔记\8_无人值守\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E28EF0-6374-4A8A-B528-417F79F6D5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FACD43-6120-4262-BB2B-82F7BCA568CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="相关问题" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="131">
   <si>
     <t>编号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -724,6 +724,14 @@
   </si>
   <si>
     <t>已完成，待测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>预约设置新增，如果现在默认选项下填好时间，但是又改为停运规则，会把那个时间数据带过来</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前端问题</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -773,18 +781,19 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>查询所有有效id，组装数据；
+      <t xml:space="preserve">查询所有有效id，组装数据；
 2，更新预约设置表，打上当天日期，防止重复生成；
 待优化项：
 获取有效设置仍然是遍历获取每个煤厂的。
 优化思路：
 从最新增或预约设置处着手，判断哪个是唯一有效的预约设置，看是否可以增加标记，使唯一有效的设置数据打上“1”，其它都设置为“0”。
-后期获取有效设置时根据标记获取，注意还要判断预约设置的有效时间。</t>
+后期获取有效设置时根据标记获取，注意还要判断预约设置的有效时间。
+</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>预约设置新增，如果现在默认选项下填好时间，但是又改为停运规则，会把那个时间数据带过来</t>
+    <t>左边分析做法错误，没找到真正原因。真正原因是非操作数据库的代码中有死循环，导致事务超时。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -997,7 +1006,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1048,44 +1057,53 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1094,6 +1112,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1102,44 +1132,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1427,15 +1439,15 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.83203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="25.58203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.58203125" customWidth="1"/>
+    <col min="2" max="2" width="52.875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="25.625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1449,8 +1461,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="31">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1459,16 +1471,16 @@
       <c r="C2" s="2"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="108" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18"/>
+    <row r="3" spans="1:4" ht="108" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="31"/>
       <c r="B3" s="3" t="s">
         <v>107</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18">
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="31">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1477,16 +1489,16 @@
       <c r="C4" s="2"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="31"/>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18">
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="31">
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1495,16 +1507,16 @@
       <c r="C6" s="2"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
+    <row r="7" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="31"/>
       <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18">
+    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="31">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1513,16 +1525,16 @@
       <c r="C8" s="2"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
+    <row r="9" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="31"/>
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="19">
+    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="21">
         <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1531,15 +1543,15 @@
       <c r="C10" s="2"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="56" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
+    <row r="11" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+      <c r="A11" s="22"/>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19">
+    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="21">
         <v>6</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1548,16 +1560,16 @@
       <c r="C12" s="2"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" ht="56" x14ac:dyDescent="0.3">
-      <c r="A13" s="20"/>
+    <row r="13" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+      <c r="A13" s="22"/>
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19">
+    <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="21">
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1566,33 +1578,33 @@
       <c r="C14" s="2"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="71.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
+    <row r="15" spans="1:4" ht="71.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="22"/>
       <c r="B15" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="19">
+    <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="21">
         <v>8</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="21" t="s">
         <v>98</v>
       </c>
       <c r="D16" s="29"/>
     </row>
-    <row r="17" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
+    <row r="17" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="22"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="20"/>
+      <c r="C17" s="22"/>
       <c r="D17" s="30"/>
     </row>
-    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="23">
         <v>9</v>
       </c>
@@ -1604,7 +1616,7 @@
       </c>
       <c r="D18" s="27"/>
     </row>
-    <row r="19" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="24"/>
       <c r="B19" s="16" t="s">
         <v>97</v>
@@ -1612,27 +1624,32 @@
       <c r="C19" s="26"/>
       <c r="D19" s="28"/>
     </row>
-    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="19">
+    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="21">
         <v>10</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="21"/>
-    </row>
-    <row r="21" spans="1:4" ht="102" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="19"/>
+    </row>
+    <row r="21" spans="1:4" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="22"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="22"/>
-    </row>
-    <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="20"/>
+    </row>
+    <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A15"/>
@@ -1644,11 +1661,6 @@
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="D16:D17"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1664,23 +1676,23 @@
       <selection activeCell="D23" sqref="D23:D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.83203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="59.875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.875" style="5" customWidth="1"/>
     <col min="4" max="4" width="25.25" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-    </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+    </row>
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1694,8 +1706,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="33">
+    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="40">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1704,8 +1716,8 @@
       <c r="C3" s="6"/>
       <c r="D3" s="13"/>
     </row>
-    <row r="4" spans="1:4" ht="154" x14ac:dyDescent="0.3">
-      <c r="A4" s="34"/>
+    <row r="4" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="41"/>
       <c r="B4" s="3" t="s">
         <v>37</v>
       </c>
@@ -1716,237 +1728,255 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36">
+    <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="38">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="37" t="s">
+      <c r="C5" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="32" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="36"/>
+    <row r="6" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="38"/>
       <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="38"/>
-    </row>
-    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="36">
+      <c r="C6" s="35"/>
+      <c r="D6" s="33"/>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="38">
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="39"/>
-    </row>
-    <row r="8" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="36"/>
+      <c r="D7" s="43"/>
+    </row>
+    <row r="8" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="38"/>
       <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="40"/>
-    </row>
-    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="36">
+      <c r="D8" s="44"/>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="38">
         <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="140" x14ac:dyDescent="0.3">
-      <c r="A10" s="36"/>
+    <row r="10" spans="1:4" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="38"/>
       <c r="B10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="42"/>
-    </row>
-    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="33">
+      <c r="C10" s="35"/>
+      <c r="D10" s="37"/>
+    </row>
+    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="40">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="37"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="34"/>
+      <c r="C11" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="32"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="41"/>
       <c r="B12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="38"/>
-    </row>
-    <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="33">
+      <c r="C12" s="35"/>
+      <c r="D12" s="33"/>
+    </row>
+    <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="40">
         <v>6</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="37"/>
-    </row>
-    <row r="14" spans="1:4" ht="28" x14ac:dyDescent="0.3">
-      <c r="A14" s="34"/>
+      <c r="C13" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="32"/>
+    </row>
+    <row r="14" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="41"/>
       <c r="B14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="38"/>
-    </row>
-    <row r="15" spans="1:4" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="33">
+      <c r="C14" s="35"/>
+      <c r="D14" s="33"/>
+    </row>
+    <row r="15" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="40">
         <v>7</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="37" t="s">
+      <c r="C15" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="32" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="50.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="34"/>
+    <row r="16" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="41"/>
       <c r="B16" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="38"/>
-    </row>
-    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="33">
+      <c r="C16" s="35"/>
+      <c r="D16" s="33"/>
+    </row>
+    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="40">
         <v>8</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="37" t="s">
+      <c r="C17" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="32" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="49" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="34"/>
+    <row r="18" spans="1:4" ht="48.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="41"/>
       <c r="B18" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="38"/>
-    </row>
-    <row r="19" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="36">
+      <c r="C18" s="35"/>
+      <c r="D18" s="33"/>
+    </row>
+    <row r="19" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="38">
         <v>9</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="37"/>
-    </row>
-    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="36"/>
+      <c r="C19" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="32"/>
+    </row>
+    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="38"/>
       <c r="B20" s="8"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="38"/>
-    </row>
-    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="36">
+      <c r="C20" s="35"/>
+      <c r="D20" s="33"/>
+    </row>
+    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="38">
         <v>10</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="37">
+      <c r="C21" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="32">
         <v>44995</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="84" x14ac:dyDescent="0.3">
-      <c r="A22" s="36"/>
+    <row r="22" spans="1:4" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="38"/>
       <c r="B22" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="32"/>
-      <c r="D22" s="38"/>
-    </row>
-    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="43">
+      <c r="C22" s="35"/>
+      <c r="D22" s="33"/>
+    </row>
+    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="39">
         <v>11</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="37" t="s">
+      <c r="C23" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="32" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="42" x14ac:dyDescent="0.3">
-      <c r="A24" s="43"/>
+    <row r="24" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="39"/>
       <c r="B24" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="32"/>
-      <c r="D24" s="38"/>
-    </row>
-    <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="36">
+      <c r="C24" s="35"/>
+      <c r="D24" s="33"/>
+    </row>
+    <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="38">
         <v>12</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25" s="37"/>
-    </row>
-    <row r="26" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="36"/>
+      <c r="C25" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="32"/>
+    </row>
+    <row r="26" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="38"/>
       <c r="B26" s="10"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="38"/>
-    </row>
-    <row r="27" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="33"/>
+    </row>
+    <row r="27" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D8"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="C9:C10"/>
@@ -1963,24 +1993,6 @@
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="A15:A16"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1996,23 +2008,23 @@
       <selection activeCell="D29" sqref="D29:D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.08203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="57.125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.875" style="5" customWidth="1"/>
     <col min="4" max="4" width="25.25" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-    </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+    </row>
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2026,319 +2038,289 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28" x14ac:dyDescent="0.3">
-      <c r="A3" s="33">
+    <row r="3" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="40">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="39" t="s">
+      <c r="C3" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="43" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="34"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="41"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="40"/>
-    </row>
-    <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36">
+      <c r="C4" s="35"/>
+      <c r="D4" s="44"/>
+    </row>
+    <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="38">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="37"/>
-    </row>
-    <row r="6" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="36"/>
+      <c r="C5" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="32"/>
+    </row>
+    <row r="6" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="38"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="38"/>
-    </row>
-    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="36">
+      <c r="C6" s="35"/>
+      <c r="D6" s="33"/>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="38">
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="39"/>
-    </row>
-    <row r="8" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="36"/>
+      <c r="C7" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="43"/>
+    </row>
+    <row r="8" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="38"/>
       <c r="B8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="40"/>
-    </row>
-    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="36">
+      <c r="C8" s="35"/>
+      <c r="D8" s="44"/>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="38">
         <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="41"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="36"/>
+      <c r="C9" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="36"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="38"/>
       <c r="B10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="42"/>
-    </row>
-    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="33">
+      <c r="C10" s="35"/>
+      <c r="D10" s="37"/>
+    </row>
+    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="40">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="37"/>
-    </row>
-    <row r="12" spans="1:4" ht="154" x14ac:dyDescent="0.3">
-      <c r="A12" s="34"/>
+      <c r="C11" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="32"/>
+    </row>
+    <row r="12" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="41"/>
       <c r="B12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="38"/>
-    </row>
-    <row r="13" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="33">
+      <c r="C12" s="35"/>
+      <c r="D12" s="33"/>
+    </row>
+    <row r="13" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="40">
         <v>6</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="37"/>
-    </row>
-    <row r="14" spans="1:4" ht="46" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="34"/>
+      <c r="C13" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="32"/>
+    </row>
+    <row r="14" spans="1:4" ht="45.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="41"/>
       <c r="B14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="38"/>
-    </row>
-    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="33">
+      <c r="C14" s="35"/>
+      <c r="D14" s="33"/>
+    </row>
+    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="40">
         <v>7</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="37" t="s">
+      <c r="C15" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="32" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="50.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="34"/>
+    <row r="16" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="41"/>
       <c r="B16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="38"/>
-    </row>
-    <row r="17" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="33">
+      <c r="C16" s="35"/>
+      <c r="D16" s="33"/>
+    </row>
+    <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="40">
         <v>8</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="37"/>
-    </row>
-    <row r="18" spans="1:4" ht="42" x14ac:dyDescent="0.3">
-      <c r="A18" s="44"/>
+      <c r="C17" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="32"/>
+    </row>
+    <row r="18" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="45"/>
       <c r="B18" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="45"/>
-      <c r="D18" s="38"/>
-    </row>
-    <row r="19" spans="1:4" ht="168" x14ac:dyDescent="0.3">
-      <c r="A19" s="44"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="33"/>
+    </row>
+    <row r="19" spans="1:4" ht="171" x14ac:dyDescent="0.2">
+      <c r="A19" s="45"/>
       <c r="B19" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="45"/>
+      <c r="C19" s="46"/>
       <c r="D19" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="76" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="34"/>
+    <row r="20" spans="1:4" ht="75.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="41"/>
       <c r="B20" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="32"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="36.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="33">
+    <row r="21" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="40">
         <v>9</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="37" t="s">
+      <c r="C21" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="32" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="44.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="34"/>
+    <row r="22" spans="1:4" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="41"/>
       <c r="B22" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="32"/>
-      <c r="D22" s="38"/>
-    </row>
-    <row r="23" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="33">
+      <c r="C22" s="35"/>
+      <c r="D22" s="33"/>
+    </row>
+    <row r="23" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="40">
         <v>10</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="37"/>
-    </row>
-    <row r="24" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="34"/>
+      <c r="C23" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="32"/>
+    </row>
+    <row r="24" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="41"/>
       <c r="B24" s="8"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="38"/>
-    </row>
-    <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="33">
+      <c r="C24" s="35"/>
+      <c r="D24" s="33"/>
+    </row>
+    <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="40">
         <v>11</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25" s="37"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="34"/>
+      <c r="C25" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="32"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="41"/>
       <c r="B26" s="10"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="38"/>
-    </row>
-    <row r="27" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="33">
+      <c r="C26" s="35"/>
+      <c r="D26" s="33"/>
+    </row>
+    <row r="27" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="40">
         <v>12</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="37"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="34"/>
+      <c r="C27" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="32"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="41"/>
       <c r="B28" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="32"/>
-      <c r="D28" s="38"/>
-    </row>
-    <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="33">
+      <c r="C28" s="35"/>
+      <c r="D28" s="33"/>
+    </row>
+    <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="40">
         <v>13</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C29" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="37" t="s">
+      <c r="C29" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="32" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="34"/>
+    <row r="30" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="41"/>
       <c r="B30" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="32"/>
-      <c r="D30" s="38"/>
-    </row>
-    <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="33"/>
+    </row>
+    <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:A4"/>
@@ -2349,6 +2331,36 @@
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2364,23 +2376,23 @@
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.25" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="79" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="14.875" style="5" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-    </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+    </row>
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2394,202 +2406,202 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="33">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="40">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="31" t="s">
+      <c r="C3" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="34" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34"/>
+    <row r="4" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="41"/>
       <c r="B4" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-    </row>
-    <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36">
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+    </row>
+    <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="38">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="31"/>
-    </row>
-    <row r="6" spans="1:4" ht="140" x14ac:dyDescent="0.3">
-      <c r="A6" s="36"/>
+      <c r="C5" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="34"/>
+    </row>
+    <row r="6" spans="1:4" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="38"/>
       <c r="B6" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-    </row>
-    <row r="7" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="36">
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+    </row>
+    <row r="7" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="38">
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="31"/>
-    </row>
-    <row r="8" spans="1:4" ht="56" x14ac:dyDescent="0.3">
-      <c r="A8" s="36"/>
+      <c r="C7" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="34"/>
+    </row>
+    <row r="8" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+      <c r="A8" s="38"/>
       <c r="B8" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-    </row>
-    <row r="9" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="33">
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+    </row>
+    <row r="9" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="40">
         <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="31"/>
-    </row>
-    <row r="10" spans="1:4" ht="111" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="34"/>
+      <c r="C9" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="34"/>
+    </row>
+    <row r="10" spans="1:4" ht="111" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="41"/>
       <c r="B10" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-    </row>
-    <row r="11" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="36">
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+    </row>
+    <row r="11" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="38">
         <v>5</v>
       </c>
       <c r="B11" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="46" t="s">
+      <c r="C11" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="48" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="231" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="36"/>
+    <row r="12" spans="1:4" ht="231" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="38"/>
       <c r="B12" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="42"/>
-    </row>
-    <row r="13" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="36">
+      <c r="C12" s="35"/>
+      <c r="D12" s="37"/>
+    </row>
+    <row r="13" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="38">
         <v>6</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="33"/>
-    </row>
-    <row r="14" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="36"/>
+      <c r="C13" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="40"/>
+    </row>
+    <row r="14" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="38"/>
       <c r="B14" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="34"/>
-    </row>
-    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="36">
+      <c r="C14" s="35"/>
+      <c r="D14" s="41"/>
+    </row>
+    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="38">
         <v>7</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="44" t="s">
+      <c r="C15" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="45" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="119.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="36"/>
+    <row r="16" spans="1:4" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="38"/>
       <c r="B16" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="34"/>
-    </row>
-    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36">
+      <c r="C16" s="35"/>
+      <c r="D16" s="41"/>
+    </row>
+    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="38">
         <v>8</v>
       </c>
       <c r="B17" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="41" t="s">
+      <c r="C17" s="34"/>
+      <c r="D17" s="36" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="250.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="36"/>
+    <row r="18" spans="1:4" ht="250.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="38"/>
       <c r="B18" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="42"/>
-    </row>
-    <row r="19" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="33">
+      <c r="C18" s="35"/>
+      <c r="D18" s="37"/>
+    </row>
+    <row r="19" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="40">
         <v>9</v>
       </c>
       <c r="B19" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="31"/>
-    </row>
-    <row r="20" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="44"/>
+      <c r="D19" s="34"/>
+    </row>
+    <row r="20" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="45"/>
       <c r="B20" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="45"/>
-      <c r="D20" s="32"/>
-    </row>
-    <row r="21" spans="1:4" ht="210" x14ac:dyDescent="0.3">
-      <c r="A21" s="44"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="35"/>
+    </row>
+    <row r="21" spans="1:4" ht="213.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="45"/>
       <c r="B21" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="45"/>
+      <c r="C21" s="46"/>
       <c r="D21" s="17"/>
     </row>
-    <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="36">
+    <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="38">
         <v>10</v>
       </c>
       <c r="B22" s="9" t="s">
@@ -2600,95 +2612,120 @@
       </c>
       <c r="D22" s="47"/>
     </row>
-    <row r="23" spans="1:4" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="36"/>
+    <row r="23" spans="1:4" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="38"/>
       <c r="B23" s="10" t="s">
         <v>114</v>
       </c>
       <c r="C23" s="47"/>
       <c r="D23" s="47"/>
     </row>
-    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="36"/>
+    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="38"/>
       <c r="B24" s="10"/>
       <c r="C24" s="47"/>
       <c r="D24" s="47"/>
     </row>
-    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="36"/>
+    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="38"/>
       <c r="B25" s="10"/>
       <c r="C25" s="47"/>
       <c r="D25" s="47"/>
     </row>
-    <row r="26" spans="1:4" ht="36.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="33"/>
+    <row r="26" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="40"/>
       <c r="B26" s="10"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="37"/>
-    </row>
-    <row r="27" spans="1:4" ht="44.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="32"/>
+    </row>
+    <row r="27" spans="1:4" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="41"/>
       <c r="B27" s="10"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="38"/>
-    </row>
-    <row r="28" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="33"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="33"/>
+    </row>
+    <row r="28" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="40"/>
       <c r="B28" s="9"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-    </row>
-    <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="34"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+    </row>
+    <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="41"/>
       <c r="B29" s="8"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-    </row>
-    <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="33"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+    </row>
+    <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="40"/>
       <c r="B30" s="9"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="41"/>
       <c r="B31" s="10"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-    </row>
-    <row r="32" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="33"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+    </row>
+    <row r="32" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="40"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="34"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="41"/>
       <c r="B33" s="10"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-    </row>
-    <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="33"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
+    </row>
+    <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="40"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-    </row>
-    <row r="35" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+    </row>
+    <row r="35" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="41"/>
       <c r="B35" s="10"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-    </row>
-    <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+    </row>
+    <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="D28:D29"/>
@@ -2701,37 +2738,12 @@
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="D32:D33"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2744,26 +2756,26 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.25" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="73.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="14.875" style="5" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-    </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+    </row>
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2777,25 +2789,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="33">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="40">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="31"/>
-    </row>
-    <row r="4" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34"/>
+      <c r="C3" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="34"/>
+    </row>
+    <row r="4" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="41"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-    </row>
-    <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+    </row>
+    <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="23">
         <v>2</v>
       </c>
@@ -2805,172 +2817,172 @@
       <c r="C5" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="34">
         <v>45040</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="84" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A6" s="24"/>
       <c r="B6" s="3" t="s">
         <v>102</v>
       </c>
       <c r="C6" s="26"/>
-      <c r="D6" s="32"/>
-    </row>
-    <row r="7" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="36">
+      <c r="D6" s="35"/>
+    </row>
+    <row r="7" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="38">
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="31"/>
-    </row>
-    <row r="8" spans="1:4" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="36"/>
+      <c r="C7" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="34"/>
+    </row>
+    <row r="8" spans="1:4" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="38"/>
       <c r="B8" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-    </row>
-    <row r="9" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="33">
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+    </row>
+    <row r="9" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="40">
         <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C9" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="31"/>
-    </row>
-    <row r="10" spans="1:4" ht="111" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="34"/>
+      <c r="C9" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="34"/>
+    </row>
+    <row r="10" spans="1:4" ht="111" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="41"/>
       <c r="B10" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-    </row>
-    <row r="11" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="36">
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+    </row>
+    <row r="11" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="38">
         <v>5</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C11" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="46"/>
-    </row>
-    <row r="12" spans="1:4" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="36"/>
+      <c r="C11" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="48"/>
+    </row>
+    <row r="12" spans="1:4" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="38"/>
       <c r="B12" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="42"/>
-    </row>
-    <row r="13" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="36">
+      <c r="C12" s="35"/>
+      <c r="D12" s="37"/>
+    </row>
+    <row r="13" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="38">
         <v>6</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C13" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="33"/>
-    </row>
-    <row r="14" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="36"/>
+      <c r="C13" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="40"/>
+    </row>
+    <row r="14" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="38"/>
       <c r="B14" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="34"/>
-    </row>
-    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="36">
+      <c r="C14" s="35"/>
+      <c r="D14" s="41"/>
+    </row>
+    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="38">
         <v>7</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="D15" s="44"/>
-    </row>
-    <row r="16" spans="1:4" ht="119.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="36"/>
+      <c r="D15" s="45"/>
+    </row>
+    <row r="16" spans="1:4" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="38"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="34"/>
-    </row>
-    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36">
+      <c r="C16" s="35"/>
+      <c r="D16" s="41"/>
+    </row>
+    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="38">
         <v>8</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="33"/>
-    </row>
-    <row r="18" spans="1:4" ht="72.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="36"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="40"/>
+    </row>
+    <row r="18" spans="1:4" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="38"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="34"/>
-    </row>
-    <row r="19" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="33">
+      <c r="C18" s="35"/>
+      <c r="D18" s="41"/>
+    </row>
+    <row r="19" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="40">
         <v>9</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="C19" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="31" t="s">
+      <c r="C19" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="34" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="139" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="44"/>
+    <row r="20" spans="1:4" ht="138.94999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="45"/>
       <c r="B20" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C20" s="45"/>
-      <c r="D20" s="32"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="33">
+      <c r="C20" s="46"/>
+      <c r="D20" s="35"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="40">
         <v>10</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>122</v>
       </c>
       <c r="C21" s="47"/>
-      <c r="D21" s="31"/>
-    </row>
-    <row r="22" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="34"/>
+      <c r="D21" s="34"/>
+    </row>
+    <row r="22" spans="1:4" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="41"/>
       <c r="B22" s="3"/>
       <c r="C22" s="47"/>
-      <c r="D22" s="32"/>
-    </row>
-    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="36">
+      <c r="D22" s="35"/>
+    </row>
+    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="38">
         <v>11</v>
       </c>
       <c r="B23" s="9" t="s">
@@ -2979,119 +2991,132 @@
       <c r="C23" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="D23" s="47"/>
-    </row>
-    <row r="24" spans="1:4" ht="168" x14ac:dyDescent="0.3">
-      <c r="A24" s="36"/>
-      <c r="B24" s="48" t="s">
-        <v>127</v>
+      <c r="D23" s="47" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="225" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="38"/>
+      <c r="B24" s="18" t="s">
+        <v>129</v>
       </c>
       <c r="C24" s="47"/>
       <c r="D24" s="47"/>
     </row>
-    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="36">
+    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="38">
         <v>12</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>124</v>
       </c>
       <c r="C25" s="47"/>
-      <c r="D25" s="47"/>
-    </row>
-    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="36"/>
+      <c r="D25" s="49" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="38"/>
       <c r="B26" s="10" t="s">
         <v>125</v>
       </c>
       <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-    </row>
-    <row r="27" spans="1:4" ht="36.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="33">
+      <c r="D26" s="49"/>
+    </row>
+    <row r="27" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="40">
         <v>13</v>
       </c>
       <c r="B27" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" s="34"/>
+      <c r="D27" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="37"/>
-    </row>
-    <row r="28" spans="1:4" ht="44.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="34"/>
+    </row>
+    <row r="28" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="41"/>
       <c r="B28" s="10"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="38"/>
-    </row>
-    <row r="29" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="33"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="33"/>
+    </row>
+    <row r="29" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="40"/>
       <c r="B29" s="9"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-    </row>
-    <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+    </row>
+    <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="41"/>
       <c r="B30" s="8"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-    </row>
-    <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="33"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+    </row>
+    <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="40"/>
       <c r="B31" s="9"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="41"/>
       <c r="B32" s="10"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-    </row>
-    <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="33"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+    </row>
+    <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="40"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="41"/>
       <c r="B34" s="10"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
-    </row>
-    <row r="35" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="33"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+    </row>
+    <row r="35" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="40"/>
       <c r="B35" s="9"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-    </row>
-    <row r="36" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+    </row>
+    <row r="36" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="41"/>
       <c r="B36" s="10"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-    </row>
-    <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+    </row>
+    <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="A23:A24"/>
@@ -3101,34 +3126,27 @@
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C21:C22"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="52" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="50" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>